<commit_message>
data pushed to excel
</commit_message>
<xml_diff>
--- a/ESheet_second.xlsx
+++ b/ESheet_second.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,22 +436,17 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Itemname</t>
+          <t>ValidUntil</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Desc</t>
+          <t>Item_name</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Price</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>ValidUntil</t>
         </is>
       </c>
     </row>
@@ -466,7 +461,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dish drainer</t>
+          <t>Waste bin</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -474,9 +469,344 @@
           <t>3</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Scented tealight</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>18-piece cutlery set</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Cushion</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Storage box with lid</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Shower curtain</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Hook</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Storage box with lid</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Cushion cover</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
         <is>
           <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>White wine glass</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Rug, low pile</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Scented candle in glass</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Rug, low pile</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Hook</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Mirror</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Throw</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Throw</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Price valid until 28 Mar</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Block-out curtains, 1 pair</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>9</t>
         </is>
       </c>
     </row>

</xml_diff>